<commit_message>
First few data files
</commit_message>
<xml_diff>
--- a/Data/glof_after1979.xlsx
+++ b/Data/glof_after1979.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\Felix_Internship_NTNU\glofData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/erikkus_cicero_oslo_no/Documents/Documents/00000 - Primary Research/GLOF - Glacial Lake Outflow/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D5EEA-F17C-4F74-A8C1-5F81C5599B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9E7D5EEA-F17C-4F74-A8C1-5F81C5599B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D82BB93C-B098-42C9-92F6-36C5DEDBC2BB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-9585" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1389,7 +1389,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1694,22 +1694,22 @@
   <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="4" width="19" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.90625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="129" customWidth="1"/>
-    <col min="7" max="7" width="24.54296875" style="129" customWidth="1"/>
-    <col min="8" max="8" width="22.1796875" style="129" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="129" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="129" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="129" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="77" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="77" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>18</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="165" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" s="165" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="165" t="s">
         <v>29</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="74" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>30</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>30</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>30</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>30</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="160" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" s="160" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="160" t="s">
         <v>12</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" s="71" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="71" t="s">
         <v>32</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>32</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>32</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>32</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="155" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" s="155" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="155" t="s">
         <v>34</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="151" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" s="151" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="151" t="s">
         <v>87</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="65" t="s">
         <v>5</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>5</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>5</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>5</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>5</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>5</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>5</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>5</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>5</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>5</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
         <v>26</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>26</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>26</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="53" t="s">
         <v>11</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="56" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="56" t="s">
         <v>43</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="59" t="s">
         <v>42</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
         <v>20</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>20</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>20</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>20</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>20</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>20</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="47" t="s">
         <v>39</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>39</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>39</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>39</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>39</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>39</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>39</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>39</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
         <v>39</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
         <v>39</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>39</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="80" t="s">
         <v>13</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
         <v>13</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>13</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>13</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
         <v>13</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
         <v>13</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
         <v>13</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
         <v>13</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
         <v>13</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
         <v>13</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
         <v>13</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
         <v>13</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
         <v>13</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
         <v>13</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="83" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="83" t="s">
         <v>28</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>28</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>28</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>28</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="86" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="86" t="s">
         <v>45</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="68" t="s">
         <v>36</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="89" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="89" t="s">
         <v>38</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
         <v>38</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="108" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="108" t="s">
         <v>24</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="111" t="s">
         <v>24</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="92" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="92" t="s">
         <v>44</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="104" t="s">
         <v>15</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="42" t="s">
         <v>15</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="42" t="s">
         <v>15</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="42" t="s">
         <v>15</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="42" t="s">
         <v>15</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="42" t="s">
         <v>15</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="42" t="s">
         <v>15</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="42" t="s">
         <v>15</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="95" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" s="95" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="95" t="s">
         <v>35</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="36" t="s">
         <v>35</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
         <v>35</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="36" t="s">
         <v>35</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>35</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="98" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="98" t="s">
         <v>22</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="101" t="s">
         <v>27</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="39" t="s">
         <v>27</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="39" t="s">
         <v>27</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="39" t="s">
         <v>27</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="39" t="s">
         <v>27</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="104" t="s">
         <v>37</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="42" t="s">
         <v>37</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="42" t="s">
         <v>37</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="42" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
New GLOF event in raw data, some server-side script improvements, and a new data extraction
</commit_message>
<xml_diff>
--- a/Data/glof_after1979.xlsx
+++ b/Data/glof_after1979.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cicero-my.sharepoint.com/personal/erikkus_cicero_oslo_no/Documents/Documents/00000 - Primary Research/GLOF - Glacial Lake Outflow/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9E7D5EEA-F17C-4F74-A8C1-5F81C5599B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D82BB93C-B098-42C9-92F6-36C5DEDBC2BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E25DED-9D4C-4F8C-93A0-D7FAFBF4F146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-9585" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-8595" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="239">
   <si>
     <t>Glacier name</t>
   </si>
@@ -734,6 +734,9 @@
   </si>
   <si>
     <t>07.03.2023-05.07.2023</t>
+  </si>
+  <si>
+    <t>28.12.2024-27.04.2025</t>
   </si>
 </sst>
 </file>
@@ -1691,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,68 +3637,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="80" t="s">
+    <row r="65" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="25">
+        <v>45774</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E65" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="G65" s="121" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="121" t="s">
+        <v>62</v>
+      </c>
+      <c r="I65" s="26">
+        <v>2025</v>
+      </c>
+      <c r="J65" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="80" t="s">
+      <c r="B66" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="81">
+      <c r="C66" s="81">
         <v>37139</v>
       </c>
-      <c r="D65" s="81" t="s">
+      <c r="D66" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="E65" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="F65" s="141" t="s">
+      <c r="E66" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="141" t="s">
         <v>56</v>
       </c>
-      <c r="G65" s="141" t="s">
-        <v>57</v>
-      </c>
-      <c r="H65" s="122" t="s">
-        <v>63</v>
-      </c>
-      <c r="I65" s="82">
-        <v>2001</v>
-      </c>
-      <c r="J65" s="80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="28">
-        <v>38593</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E66" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="F66" s="122" t="s">
-        <v>56</v>
-      </c>
-      <c r="G66" s="122" t="s">
+      <c r="G66" s="141" t="s">
         <v>57</v>
       </c>
       <c r="H66" s="122" t="s">
         <v>63</v>
       </c>
-      <c r="I66" s="29">
-        <v>2005</v>
-      </c>
-      <c r="J66" s="27" t="s">
-        <v>8</v>
+      <c r="I66" s="82">
+        <v>2001</v>
+      </c>
+      <c r="J66" s="80" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3706,10 +3709,10 @@
         <v>14</v>
       </c>
       <c r="C67" s="28">
-        <v>39323</v>
+        <v>38593</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E67" s="28" t="s">
         <v>52</v>
@@ -3724,7 +3727,7 @@
         <v>63</v>
       </c>
       <c r="I67" s="29">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="J67" s="27" t="s">
         <v>8</v>
@@ -3738,10 +3741,10 @@
         <v>14</v>
       </c>
       <c r="C68" s="28">
-        <v>40062</v>
+        <v>39323</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E68" s="28" t="s">
         <v>52</v>
@@ -3756,10 +3759,10 @@
         <v>63</v>
       </c>
       <c r="I68" s="29">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="J68" s="27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3770,10 +3773,10 @@
         <v>14</v>
       </c>
       <c r="C69" s="28">
-        <v>40429</v>
+        <v>40062</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E69" s="28" t="s">
         <v>52</v>
@@ -3788,7 +3791,7 @@
         <v>63</v>
       </c>
       <c r="I69" s="29">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="J69" s="27" t="s">
         <v>7</v>
@@ -3802,10 +3805,10 @@
         <v>14</v>
       </c>
       <c r="C70" s="28">
-        <v>40808</v>
+        <v>40429</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E70" s="28" t="s">
         <v>52</v>
@@ -3820,7 +3823,7 @@
         <v>63</v>
       </c>
       <c r="I70" s="29">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="J70" s="27" t="s">
         <v>7</v>
@@ -3834,10 +3837,10 @@
         <v>14</v>
       </c>
       <c r="C71" s="28">
-        <v>41862</v>
+        <v>40808</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E71" s="28" t="s">
         <v>52</v>
@@ -3852,10 +3855,10 @@
         <v>63</v>
       </c>
       <c r="I71" s="29">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="J71" s="27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3866,10 +3869,10 @@
         <v>14</v>
       </c>
       <c r="C72" s="28">
-        <v>42641</v>
+        <v>41862</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E72" s="28" t="s">
         <v>52</v>
@@ -3884,10 +3887,10 @@
         <v>63</v>
       </c>
       <c r="I72" s="29">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="J72" s="27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3898,13 +3901,13 @@
         <v>14</v>
       </c>
       <c r="C73" s="28">
-        <v>43337</v>
+        <v>42641</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F73" s="122" t="s">
         <v>56</v>
@@ -3916,10 +3919,10 @@
         <v>63</v>
       </c>
       <c r="I73" s="29">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="J73" s="27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3930,10 +3933,10 @@
         <v>14</v>
       </c>
       <c r="C74" s="28">
-        <v>43717</v>
+        <v>43337</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E74" s="28" t="s">
         <v>53</v>
@@ -3948,10 +3951,10 @@
         <v>63</v>
       </c>
       <c r="I74" s="29">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="J74" s="27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3962,10 +3965,10 @@
         <v>14</v>
       </c>
       <c r="C75" s="28">
-        <v>44078</v>
+        <v>43717</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E75" s="28" t="s">
         <v>53</v>
@@ -3980,7 +3983,7 @@
         <v>63</v>
       </c>
       <c r="I75" s="29">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="J75" s="27" t="s">
         <v>7</v>
@@ -3994,10 +3997,10 @@
         <v>14</v>
       </c>
       <c r="C76" s="28">
-        <v>44810</v>
+        <v>44078</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E76" s="28" t="s">
         <v>53</v>
@@ -4012,7 +4015,7 @@
         <v>63</v>
       </c>
       <c r="I76" s="29">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="J76" s="27" t="s">
         <v>7</v>
@@ -4026,10 +4029,10 @@
         <v>14</v>
       </c>
       <c r="C77" s="28">
-        <v>45166</v>
+        <v>44810</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E77" s="28" t="s">
         <v>53</v>
@@ -4044,10 +4047,10 @@
         <v>63</v>
       </c>
       <c r="I77" s="29">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="J77" s="27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4058,13 +4061,13 @@
         <v>14</v>
       </c>
       <c r="C78" s="28">
-        <v>45516</v>
+        <v>45166</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F78" s="122" t="s">
         <v>56</v>
@@ -4076,68 +4079,71 @@
         <v>63</v>
       </c>
       <c r="I78" s="29">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="J78" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="83" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="83" t="s">
+    <row r="79" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="28">
+        <v>45516</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F79" s="122" t="s">
+        <v>56</v>
+      </c>
+      <c r="G79" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="H79" s="122" t="s">
+        <v>63</v>
+      </c>
+      <c r="I79" s="29">
+        <v>2024</v>
+      </c>
+      <c r="J79" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C79" s="84">
+      <c r="C80" s="84">
         <v>43304</v>
       </c>
-      <c r="D79" s="84" t="s">
+      <c r="D80" s="84" t="s">
         <v>209</v>
       </c>
-      <c r="E79" s="84" t="s">
-        <v>52</v>
-      </c>
-      <c r="F79" s="142" t="s">
+      <c r="E80" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="F80" s="142" t="s">
         <v>102</v>
       </c>
-      <c r="G79" s="142" t="s">
+      <c r="G80" s="142" t="s">
         <v>104</v>
       </c>
-      <c r="H79" s="142" t="s">
+      <c r="H80" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="I79" s="85">
+      <c r="I80" s="85">
         <v>2018</v>
       </c>
-      <c r="J79" s="83" t="s">
+      <c r="J80" s="83" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" s="31">
-        <v>43680</v>
-      </c>
-      <c r="D80" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F80" s="123" t="s">
-        <v>102</v>
-      </c>
-      <c r="G80" s="123" t="s">
-        <v>105</v>
-      </c>
-      <c r="H80" s="123" t="s">
-        <v>103</v>
-      </c>
-      <c r="I80" s="32">
-        <v>2019</v>
-      </c>
-      <c r="J80" s="30" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -4145,10 +4151,10 @@
         <v>28</v>
       </c>
       <c r="C81" s="31">
-        <v>44459</v>
+        <v>43680</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E81" s="31" t="s">
         <v>52</v>
@@ -4157,16 +4163,16 @@
         <v>102</v>
       </c>
       <c r="G81" s="123" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H81" s="123" t="s">
         <v>103</v>
       </c>
       <c r="I81" s="32">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="J81" s="30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -4174,10 +4180,10 @@
         <v>28</v>
       </c>
       <c r="C82" s="31">
-        <v>44752</v>
+        <v>44459</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E82" s="31" t="s">
         <v>52</v>
@@ -4186,286 +4192,283 @@
         <v>102</v>
       </c>
       <c r="G82" s="123" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H82" s="123" t="s">
         <v>103</v>
       </c>
       <c r="I82" s="32">
+        <v>2021</v>
+      </c>
+      <c r="J82" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="31">
+        <v>44752</v>
+      </c>
+      <c r="D83" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E83" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F83" s="123" t="s">
+        <v>102</v>
+      </c>
+      <c r="G83" s="123" t="s">
+        <v>107</v>
+      </c>
+      <c r="H83" s="123" t="s">
+        <v>103</v>
+      </c>
+      <c r="I83" s="32">
         <v>2022</v>
       </c>
-      <c r="J82" s="30" t="s">
+      <c r="J83" s="30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="86" t="s">
+    <row r="84" spans="1:10" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="B83" s="86" t="s">
+      <c r="B84" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="C83" s="87">
+      <c r="C84" s="87">
         <v>42626</v>
       </c>
-      <c r="D83" s="87" t="s">
+      <c r="D84" s="87" t="s">
         <v>213</v>
       </c>
-      <c r="E83" s="87" t="s">
-        <v>52</v>
-      </c>
-      <c r="F83" s="143" t="s">
+      <c r="E84" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="F84" s="143" t="s">
         <v>108</v>
       </c>
-      <c r="G83" s="143" t="s">
+      <c r="G84" s="143" t="s">
         <v>110</v>
       </c>
-      <c r="H83" s="143" t="s">
+      <c r="H84" s="143" t="s">
         <v>109</v>
       </c>
-      <c r="I83" s="88">
+      <c r="I84" s="88">
         <v>2016</v>
       </c>
-      <c r="J83" s="86" t="s">
+      <c r="J84" s="86" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="68" t="s">
+    <row r="85" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C84" s="69">
+      <c r="C85" s="69">
         <v>44075</v>
       </c>
-      <c r="D84" s="69" t="s">
+      <c r="D85" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="E84" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="F84" s="133" t="s">
+      <c r="E85" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="F85" s="133" t="s">
         <v>111</v>
       </c>
-      <c r="G84" s="133" t="s">
+      <c r="G85" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="H84" s="133" t="s">
+      <c r="H85" s="133" t="s">
         <v>112</v>
       </c>
-      <c r="I84" s="70">
+      <c r="I85" s="70">
         <v>2020</v>
       </c>
-      <c r="J84" s="68" t="s">
+      <c r="J85" s="68" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="89" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="89" t="s">
+    <row r="86" spans="1:10" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="90">
+      <c r="C86" s="90">
         <v>44810</v>
       </c>
-      <c r="D85" s="90" t="s">
+      <c r="D86" s="90" t="s">
         <v>206</v>
       </c>
-      <c r="E85" s="90" t="s">
-        <v>52</v>
-      </c>
-      <c r="F85" s="144" t="s">
+      <c r="E86" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="F86" s="144" t="s">
         <v>114</v>
       </c>
-      <c r="G85" s="144" t="s">
+      <c r="G86" s="144" t="s">
         <v>116</v>
       </c>
-      <c r="H85" s="144" t="s">
+      <c r="H86" s="144" t="s">
         <v>115</v>
       </c>
-      <c r="I85" s="91">
+      <c r="I86" s="91">
         <v>2022</v>
       </c>
-      <c r="J85" s="89" t="s">
+      <c r="J86" s="89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
+    <row r="87" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="34">
+      <c r="C87" s="34">
         <v>45160</v>
       </c>
-      <c r="D86" s="34" t="s">
+      <c r="D87" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="E86" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F86" s="124" t="s">
+      <c r="E87" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F87" s="124" t="s">
         <v>114</v>
       </c>
-      <c r="G86" s="124" t="s">
+      <c r="G87" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="H86" s="124" t="s">
+      <c r="H87" s="124" t="s">
         <v>115</v>
       </c>
-      <c r="I86" s="35">
+      <c r="I87" s="35">
         <v>2023</v>
       </c>
-      <c r="J86" s="33" t="s">
+      <c r="J87" s="33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="108" t="s">
+    <row r="88" spans="1:10" s="108" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="109">
+      <c r="C88" s="109">
         <v>38115</v>
       </c>
-      <c r="D87" s="109" t="s">
+      <c r="D88" s="109" t="s">
         <v>216</v>
       </c>
-      <c r="E87" s="109" t="s">
+      <c r="E88" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="F87" s="145" t="s">
+      <c r="F88" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="G87" s="145" t="s">
-        <v>59</v>
-      </c>
-      <c r="H87" s="125" t="s">
-        <v>64</v>
-      </c>
-      <c r="I87" s="110">
-        <v>2004</v>
-      </c>
-      <c r="J87" s="108" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C88" s="112">
-        <v>44876</v>
-      </c>
-      <c r="D88" s="112" t="s">
-        <v>217</v>
-      </c>
-      <c r="E88" s="112" t="s">
-        <v>53</v>
-      </c>
-      <c r="F88" s="125" t="s">
-        <v>58</v>
-      </c>
-      <c r="G88" s="125" t="s">
+      <c r="G88" s="145" t="s">
         <v>59</v>
       </c>
       <c r="H88" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="I88" s="113">
+      <c r="I88" s="110">
+        <v>2004</v>
+      </c>
+      <c r="J88" s="108" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="112">
+        <v>44876</v>
+      </c>
+      <c r="D89" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="E89" s="112" t="s">
+        <v>53</v>
+      </c>
+      <c r="F89" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="G89" s="125" t="s">
+        <v>59</v>
+      </c>
+      <c r="H89" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="I89" s="113">
         <v>2022</v>
       </c>
-      <c r="J88" s="111" t="s">
+      <c r="J89" s="111" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="92" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="92" t="s">
+    <row r="90" spans="1:10" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="C89" s="93">
+      <c r="C90" s="93">
         <v>37469</v>
       </c>
-      <c r="D89" s="93" t="s">
+      <c r="D90" s="93" t="s">
         <v>218</v>
       </c>
-      <c r="E89" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="F89" s="146" t="s">
+      <c r="E90" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="F90" s="146" t="s">
         <v>117</v>
       </c>
-      <c r="G89" s="146" t="s">
+      <c r="G90" s="146" t="s">
         <v>119</v>
       </c>
-      <c r="H89" s="146" t="s">
+      <c r="H90" s="146" t="s">
         <v>118</v>
       </c>
-      <c r="I89" s="94">
+      <c r="I90" s="94">
         <v>2002</v>
       </c>
-      <c r="J89" s="92" t="s">
+      <c r="J90" s="92" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="104" t="s">
+    <row r="91" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="B90" s="104" t="s">
+      <c r="B91" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="C90" s="105">
+      <c r="C91" s="105">
         <v>32509</v>
       </c>
-      <c r="D90" s="105" t="s">
+      <c r="D91" s="105" t="s">
         <v>219</v>
       </c>
-      <c r="E90" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="F90" s="147" t="s">
+      <c r="E91" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="F91" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="G90" s="147" t="s">
+      <c r="G91" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="H90" s="147" t="s">
+      <c r="H91" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="I90" s="106">
+      <c r="I91" s="106">
         <v>1989</v>
       </c>
-      <c r="J90" s="104" t="s">
+      <c r="J91" s="104" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="B91" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="43">
-        <v>33339</v>
-      </c>
-      <c r="D91" s="43" t="s">
-        <v>220</v>
-      </c>
-      <c r="E91" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F91" s="126" t="s">
-        <v>120</v>
-      </c>
-      <c r="G91" s="126" t="s">
-        <v>122</v>
-      </c>
-      <c r="H91" s="126" t="s">
-        <v>121</v>
-      </c>
-      <c r="I91" s="44">
-        <v>1991</v>
-      </c>
-      <c r="J91" s="42" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4476,10 +4479,10 @@
         <v>16</v>
       </c>
       <c r="C92" s="43">
-        <v>36342</v>
+        <v>33339</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>52</v>
@@ -4494,10 +4497,10 @@
         <v>121</v>
       </c>
       <c r="I92" s="44">
-        <v>1999</v>
+        <v>1991</v>
       </c>
       <c r="J92" s="42" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4508,10 +4511,10 @@
         <v>16</v>
       </c>
       <c r="C93" s="43">
-        <v>36708</v>
+        <v>36342</v>
       </c>
       <c r="D93" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E93" s="43" t="s">
         <v>52</v>
@@ -4526,7 +4529,7 @@
         <v>121</v>
       </c>
       <c r="I93" s="44">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="J93" s="42" t="s">
         <v>9</v>
@@ -4540,10 +4543,10 @@
         <v>16</v>
       </c>
       <c r="C94" s="43">
-        <v>41852</v>
+        <v>36708</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E94" s="43" t="s">
         <v>52</v>
@@ -4558,10 +4561,10 @@
         <v>121</v>
       </c>
       <c r="I94" s="44">
-        <v>2014</v>
+        <v>2000</v>
       </c>
       <c r="J94" s="42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4572,10 +4575,10 @@
         <v>16</v>
       </c>
       <c r="C95" s="43">
-        <v>42614</v>
+        <v>41852</v>
       </c>
       <c r="D95" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E95" s="43" t="s">
         <v>52</v>
@@ -4590,10 +4593,10 @@
         <v>121</v>
       </c>
       <c r="I95" s="44">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="J95" s="42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4603,11 +4606,11 @@
       <c r="B96" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="114">
-        <v>44044</v>
-      </c>
-      <c r="D96" s="114" t="s">
-        <v>225</v>
+      <c r="C96" s="43">
+        <v>42614</v>
+      </c>
+      <c r="D96" s="43" t="s">
+        <v>224</v>
       </c>
       <c r="E96" s="43" t="s">
         <v>52</v>
@@ -4622,10 +4625,10 @@
         <v>121</v>
       </c>
       <c r="I96" s="44">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="J96" s="42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -4635,11 +4638,11 @@
       <c r="B97" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="43">
-        <v>44405</v>
-      </c>
-      <c r="D97" s="43" t="s">
-        <v>226</v>
+      <c r="C97" s="114">
+        <v>44044</v>
+      </c>
+      <c r="D97" s="114" t="s">
+        <v>225</v>
       </c>
       <c r="E97" s="43" t="s">
         <v>52</v>
@@ -4654,68 +4657,71 @@
         <v>121</v>
       </c>
       <c r="I97" s="44">
+        <v>2020</v>
+      </c>
+      <c r="J97" s="42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="43">
+        <v>44405</v>
+      </c>
+      <c r="D98" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F98" s="126" t="s">
+        <v>120</v>
+      </c>
+      <c r="G98" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="H98" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="I98" s="44">
         <v>2021</v>
       </c>
-      <c r="J97" s="42" t="s">
+      <c r="J98" s="42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="95" t="s">
+    <row r="99" spans="1:10" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="96">
+      <c r="C99" s="96">
         <v>43628</v>
       </c>
-      <c r="D98" s="96" t="s">
+      <c r="D99" s="96" t="s">
         <v>227</v>
       </c>
-      <c r="E98" s="96" t="s">
-        <v>52</v>
-      </c>
-      <c r="F98" s="148" t="s">
+      <c r="E99" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="F99" s="148" t="s">
         <v>123</v>
       </c>
-      <c r="G98" s="148" t="s">
+      <c r="G99" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="H98" s="148" t="s">
+      <c r="H99" s="148" t="s">
         <v>124</v>
       </c>
-      <c r="I98" s="97">
+      <c r="I99" s="97">
         <v>2019</v>
       </c>
-      <c r="J98" s="95" t="s">
+      <c r="J99" s="95" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C99" s="37">
-        <v>44013</v>
-      </c>
-      <c r="D99" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="E99" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F99" s="127" t="s">
-        <v>123</v>
-      </c>
-      <c r="G99" s="127" t="s">
-        <v>125</v>
-      </c>
-      <c r="H99" s="127" t="s">
-        <v>124</v>
-      </c>
-      <c r="I99" s="38">
-        <v>2020</v>
-      </c>
-      <c r="J99" s="36" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4723,10 +4729,10 @@
         <v>35</v>
       </c>
       <c r="C100" s="37">
-        <v>44376</v>
+        <v>44013</v>
       </c>
       <c r="D100" s="37" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="E100" s="37" t="s">
         <v>52</v>
@@ -4741,10 +4747,10 @@
         <v>124</v>
       </c>
       <c r="I100" s="38">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="J100" s="36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4752,10 +4758,10 @@
         <v>35</v>
       </c>
       <c r="C101" s="37">
-        <v>44767</v>
+        <v>44376</v>
       </c>
       <c r="D101" s="37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E101" s="37" t="s">
         <v>52</v>
@@ -4770,10 +4776,10 @@
         <v>124</v>
       </c>
       <c r="I101" s="38">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="J101" s="36" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4781,10 +4787,10 @@
         <v>35</v>
       </c>
       <c r="C102" s="37">
-        <v>45108</v>
+        <v>44767</v>
       </c>
       <c r="D102" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E102" s="37" t="s">
         <v>52</v>
@@ -4799,99 +4805,99 @@
         <v>124</v>
       </c>
       <c r="I102" s="38">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="J102" s="36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="98" t="s">
+    <row r="103" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="37">
+        <v>45108</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="E103" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F103" s="127" t="s">
+        <v>123</v>
+      </c>
+      <c r="G103" s="127" t="s">
+        <v>125</v>
+      </c>
+      <c r="H103" s="127" t="s">
+        <v>124</v>
+      </c>
+      <c r="I103" s="38">
+        <v>2023</v>
+      </c>
+      <c r="J103" s="36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="98" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B103" s="98" t="s">
+      <c r="B104" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C103" s="99">
+      <c r="C104" s="99">
         <v>36161</v>
       </c>
-      <c r="D103" s="99" t="s">
+      <c r="D104" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="E103" s="99" t="s">
-        <v>52</v>
-      </c>
-      <c r="F103" s="149" t="s">
+      <c r="E104" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="F104" s="149" t="s">
         <v>126</v>
       </c>
-      <c r="G103" s="149" t="s">
+      <c r="G104" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="H103" s="149" t="s">
+      <c r="H104" s="149" t="s">
         <v>127</v>
       </c>
-      <c r="I103" s="100">
+      <c r="I104" s="100">
         <v>1999</v>
       </c>
-      <c r="J103" s="98" t="s">
+      <c r="J104" s="98" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="101" t="s">
+    <row r="105" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C104" s="102">
+      <c r="C105" s="102">
         <v>40391</v>
       </c>
-      <c r="D104" s="102" t="s">
+      <c r="D105" s="102" t="s">
         <v>232</v>
       </c>
-      <c r="E104" s="102" t="s">
-        <v>52</v>
-      </c>
-      <c r="F104" s="150" t="s">
+      <c r="E105" s="102" t="s">
+        <v>52</v>
+      </c>
+      <c r="F105" s="150" t="s">
         <v>129</v>
       </c>
-      <c r="G104" s="150" t="s">
+      <c r="G105" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="H104" s="150" t="s">
+      <c r="H105" s="150" t="s">
         <v>130</v>
       </c>
-      <c r="I104" s="103">
+      <c r="I105" s="103">
         <v>2010</v>
       </c>
-      <c r="J104" s="101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C105" s="40">
-        <v>41867</v>
-      </c>
-      <c r="D105" s="40" t="s">
-        <v>233</v>
-      </c>
-      <c r="E105" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="F105" s="128" t="s">
-        <v>129</v>
-      </c>
-      <c r="G105" s="128" t="s">
-        <v>131</v>
-      </c>
-      <c r="H105" s="128" t="s">
-        <v>130</v>
-      </c>
-      <c r="I105" s="41">
-        <v>2014</v>
-      </c>
-      <c r="J105" s="39" t="s">
+      <c r="J105" s="101" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4900,10 +4906,10 @@
         <v>27</v>
       </c>
       <c r="C106" s="40">
-        <v>43266</v>
+        <v>41867</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E106" s="40" t="s">
         <v>52</v>
@@ -4918,10 +4924,10 @@
         <v>130</v>
       </c>
       <c r="I106" s="41">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="J106" s="39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -4929,10 +4935,10 @@
         <v>27</v>
       </c>
       <c r="C107" s="40">
-        <v>45523</v>
+        <v>43266</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E107" s="40" t="s">
         <v>52</v>
@@ -4947,10 +4953,10 @@
         <v>130</v>
       </c>
       <c r="I107" s="41">
-        <v>2024</v>
+        <v>2018</v>
       </c>
       <c r="J107" s="39" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -4982,62 +4988,62 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="104" t="s">
+    <row r="109" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C109" s="40">
+        <v>45523</v>
+      </c>
+      <c r="D109" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E109" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F109" s="128" t="s">
+        <v>129</v>
+      </c>
+      <c r="G109" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="H109" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="I109" s="41">
+        <v>2024</v>
+      </c>
+      <c r="J109" s="39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C109" s="105">
+      <c r="C110" s="105">
         <v>42948</v>
       </c>
-      <c r="D109" s="105" t="s">
+      <c r="D110" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="E109" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="F109" s="147" t="s">
+      <c r="E110" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="F110" s="147" t="s">
         <v>132</v>
       </c>
-      <c r="G109" s="147" t="s">
+      <c r="G110" s="147" t="s">
         <v>134</v>
       </c>
-      <c r="H109" s="147" t="s">
+      <c r="H110" s="147" t="s">
         <v>133</v>
       </c>
-      <c r="I109" s="106">
+      <c r="I110" s="106">
         <v>2017</v>
       </c>
-      <c r="J109" s="104" t="s">
+      <c r="J110" s="104" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C110" s="43">
-        <v>43301</v>
-      </c>
-      <c r="D110" s="43" t="s">
-        <v>236</v>
-      </c>
-      <c r="E110" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F110" s="126" t="s">
-        <v>132</v>
-      </c>
-      <c r="G110" s="126" t="s">
-        <v>134</v>
-      </c>
-      <c r="H110" s="126" t="s">
-        <v>133</v>
-      </c>
-      <c r="I110" s="44">
-        <v>2018</v>
-      </c>
-      <c r="J110" s="42" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -5045,10 +5051,10 @@
         <v>37</v>
       </c>
       <c r="C111" s="43">
-        <v>44752</v>
+        <v>43301</v>
       </c>
       <c r="D111" s="43" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="E111" s="43" t="s">
         <v>52</v>
@@ -5063,7 +5069,7 @@
         <v>133</v>
       </c>
       <c r="I111" s="44">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="J111" s="42" t="s">
         <v>9</v>
@@ -5074,10 +5080,10 @@
         <v>37</v>
       </c>
       <c r="C112" s="43">
-        <v>45112</v>
+        <v>44752</v>
       </c>
       <c r="D112" s="43" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="E112" s="43" t="s">
         <v>52</v>
@@ -5092,15 +5098,44 @@
         <v>133</v>
       </c>
       <c r="I112" s="44">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="J112" s="42" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="113" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C113" s="43">
+        <v>45112</v>
+      </c>
+      <c r="D113" s="43" t="s">
+        <v>237</v>
+      </c>
+      <c r="E113" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F113" s="126" t="s">
+        <v>132</v>
+      </c>
+      <c r="G113" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="H113" s="126" t="s">
+        <v>133</v>
+      </c>
+      <c r="I113" s="44">
+        <v>2023</v>
+      </c>
+      <c r="J113" s="42" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A109:J112">
-    <sortCondition ref="C109:C112"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A110:J113">
+    <sortCondition ref="C110:C113"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>